<commit_message>
added the xls file
</commit_message>
<xml_diff>
--- a/git.xlsx
+++ b/git.xlsx
@@ -5,19 +5,21 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\eclipse-workspace\feb-sdet-tcs\git-demo-tcs-sdet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rames\OneDrive\Desktop\Feb2025-SDET-TCS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ACB9ED-E944-47A5-ADCC-23113881D356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4B5751-2FD8-4BC3-8450-F135632862E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configurations" sheetId="1" r:id="rId1"/>
     <sheet name="ssh keys" sheetId="2" r:id="rId2"/>
     <sheet name="initial setup" sheetId="3" r:id="rId3"/>
     <sheet name="branch" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
+    <sheet name="simultaneous work" sheetId="5" r:id="rId5"/>
+    <sheet name="conflict" sheetId="6" r:id="rId6"/>
+    <sheet name="stash" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="137">
   <si>
     <t>name</t>
   </si>
@@ -277,9 +279,6 @@
     <t>git branch c1</t>
   </si>
   <si>
-    <t>git branch c2</t>
-  </si>
-  <si>
     <t>perform the code changes</t>
   </si>
   <si>
@@ -293,13 +292,163 @@
   </si>
   <si>
     <t>git push origin c1</t>
+  </si>
+  <si>
+    <t>PR#2</t>
+  </si>
+  <si>
+    <t>PR#3</t>
+  </si>
+  <si>
+    <t>merge the PR</t>
+  </si>
+  <si>
+    <t>v1+dy</t>
+  </si>
+  <si>
+    <t>merge</t>
+  </si>
+  <si>
+    <t>v2</t>
+  </si>
+  <si>
+    <t>v1+dy ==&gt; v2</t>
+  </si>
+  <si>
+    <t>v2+dx ==&gt; v3</t>
+  </si>
+  <si>
+    <t>v3</t>
+  </si>
+  <si>
+    <t>pull the latest code change</t>
+  </si>
+  <si>
+    <t>git branch c11</t>
+  </si>
+  <si>
+    <t>git push origin c11</t>
+  </si>
+  <si>
+    <t>git branch d11</t>
+  </si>
+  <si>
+    <t>git push origin d11</t>
+  </si>
+  <si>
+    <t>PR#4</t>
+  </si>
+  <si>
+    <t>PR#5</t>
+  </si>
+  <si>
+    <t>conflict will display</t>
+  </si>
+  <si>
+    <t>pull the latest code change to main branch</t>
+  </si>
+  <si>
+    <t>apply the latest code change in side branch</t>
+  </si>
+  <si>
+    <t>git rebase main</t>
+  </si>
+  <si>
+    <t>modify the code changes</t>
+  </si>
+  <si>
+    <t>git rebase --continue</t>
+  </si>
+  <si>
+    <t>git push origin c11 -f</t>
+  </si>
+  <si>
+    <t>make the necessary code change</t>
+  </si>
+  <si>
+    <t>add the code change</t>
+  </si>
+  <si>
+    <t>git rebase continue</t>
+  </si>
+  <si>
+    <t>forcefully push the latest code changes to gh.com side branch</t>
+  </si>
+  <si>
+    <t>review and merge</t>
+  </si>
+  <si>
+    <t>v2+dx</t>
+  </si>
+  <si>
+    <t>pull the latest code changes</t>
+  </si>
+  <si>
+    <t>git branch c111</t>
+  </si>
+  <si>
+    <t>git branch d111</t>
+  </si>
+  <si>
+    <t>git push origin d111</t>
+  </si>
+  <si>
+    <t>PR#6</t>
+  </si>
+  <si>
+    <t>dy</t>
+  </si>
+  <si>
+    <t>stash the code code</t>
+  </si>
+  <si>
+    <t>git stash</t>
+  </si>
+  <si>
+    <t>git pull the latest code</t>
+  </si>
+  <si>
+    <t>rebase the main branch code to side branch</t>
+  </si>
+  <si>
+    <t>git stash pop</t>
+  </si>
+  <si>
+    <t>conflict will display here</t>
+  </si>
+  <si>
+    <t>modify the code</t>
+  </si>
+  <si>
+    <t>make the code changes</t>
+  </si>
+  <si>
+    <t>create a pr</t>
+  </si>
+  <si>
+    <t>get it reviewed and merged</t>
+  </si>
+  <si>
+    <t>git push origin c111</t>
+  </si>
+  <si>
+    <t>PR#7</t>
+  </si>
+  <si>
+    <t>pull the latest code changes to main branch</t>
+  </si>
+  <si>
+    <t>git branch d1</t>
+  </si>
+  <si>
+    <t>git push origin d1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +486,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,6 +510,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -459,7 +622,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -511,6 +674,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1185,10 +1369,10 @@
   <dimension ref="B1:L45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="12" ySplit="8" topLeftCell="M21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="8" topLeftCell="M30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,14 +2131,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{634251A5-B1EB-413C-BE80-B4142C8FA214}">
-  <dimension ref="B1:L18"/>
+  <dimension ref="B1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="12" ySplit="6" topLeftCell="M9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="topRight" activeCell="M3" sqref="M3"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,27 +2146,37 @@
     <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="2.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
     <col min="7" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
     <col min="11" max="11" width="27.42578125" customWidth="1"/>
     <col min="12" max="12" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F1" s="1"/>
       <c r="H1" s="2"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="1"/>
       <c r="H2" s="2"/>
+      <c r="J2" s="1"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="1"/>
       <c r="H3" s="2"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
       <c r="H4" s="2"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
       <c r="H5" s="2"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
@@ -2079,7 +2273,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="11"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="H10" s="5"/>
       <c r="I10" s="4"/>
       <c r="J10" s="11"/>
       <c r="K10" s="4"/>
@@ -2094,7 +2288,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
+      <c r="H11" s="6"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -2113,12 +2307,12 @@
       <c r="E12" s="4"/>
       <c r="F12" s="11"/>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="4"/>
       <c r="J12" s="11"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4" t="s">
-        <v>82</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -2128,7 +2322,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -2139,19 +2333,19 @@
         <v>3</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="H14" s="5"/>
       <c r="I14" s="4"/>
       <c r="J14" s="11"/>
       <c r="K14" s="4" t="s">
-        <v>85</v>
+        <v>121</v>
       </c>
       <c r="L14" s="4"/>
     </row>
@@ -2168,7 +2362,7 @@
       </c>
       <c r="F15" s="11"/>
       <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="4"/>
       <c r="J15" s="11"/>
       <c r="K15" s="4" t="s">
@@ -2185,15 +2379,15 @@
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F16" s="11"/>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="5"/>
       <c r="I16" s="4"/>
       <c r="J16" s="11"/>
       <c r="K16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L16" s="4"/>
     </row>
@@ -2206,19 +2400,19 @@
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
         <v>28</v>
       </c>
       <c r="J17" s="11"/>
       <c r="K17" s="4" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="L17" s="4"/>
     </row>
@@ -2227,21 +2421,1532 @@
         <v>7</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="11"/>
       <c r="G18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H18" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="26">
+        <v>8</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L23" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>9</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="K6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D70F3E6-3BF4-4FD7-9966-6E9D9B053D56}">
+  <dimension ref="B1:L37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+    <col min="7" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="25"/>
+      <c r="F1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="25"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="25"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="25"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="25"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>4</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>7</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="26">
+        <v>8</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="H22" s="5"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>9</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="11"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+    </row>
+    <row r="26" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>10</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>11</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>12</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="4">
+        <v>13</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>14</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H32" s="5"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="11"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>15</v>
+      </c>
+      <c r="C34" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I34" s="4"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="11"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>16</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="11"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="K6:L6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A77EAFE5-5466-48AD-82EF-D4192AB15F03}">
+  <dimension ref="B1:L41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="2.42578125" customWidth="1"/>
+    <col min="7" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" customWidth="1"/>
+    <col min="12" max="12" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C1" s="25"/>
+      <c r="F1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C2" s="25"/>
+      <c r="F2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="25"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="2"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C4" s="25"/>
+      <c r="F4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="25"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="2"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="20"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="20"/>
+    </row>
+    <row r="7" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="11"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="11"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>2</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>3</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>4</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>5</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>6</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="11"/>
+      <c r="K17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>7</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="11"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="11"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="26">
+        <v>8</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>9</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>10</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="11"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+    </row>
+    <row r="27" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>11</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="11"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="4">
+        <v>12</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="11"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="11"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>13</v>
+      </c>
+      <c r="C33" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="11"/>
+      <c r="G36" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="5"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="H37" s="5"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="11"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B39" s="11"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="11"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>